<commit_message>
Alerts test data.(Danger and Warning).
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/suitecorporateLens/testdata/CorporateLensTestData-Alerts.xlsx
+++ b/Excelens_Trunk/src/com/proj/suitecorporateLens/testdata/CorporateLensTestData-Alerts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excelens_JWS\Excelens_Trunk_Jul122017\src\com\proj\suitecorporateLens\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_EXCL_JUL\Excelens_Trunk\src\com\proj\suitecorporateLens\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>RefID</t>
   </si>
   <si>
-    <t>LAT-100</t>
-  </si>
-  <si>
-    <t>LAT-92</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -61,12 +55,27 @@
   </si>
   <si>
     <t>Monthly Leaves -Automation</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>MistyRose</t>
+  </si>
+  <si>
+    <t>OldLace</t>
+  </si>
+  <si>
+    <t>LAT-137</t>
+  </si>
+  <si>
+    <t>LAT-138</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -461,11 +470,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -473,58 +480,68 @@
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>